<commit_message>
build(dependencies): 添加 Netlify 函数和 Day.js 依赖
- 在 package.json 中添加 @netlify/functions 和 dayjs 依赖
- 更新 xlsxToJson.js 文件，过滤掉空标签的项目
- 在 pnpm-lock.yaml 中添加相关依赖的版本信息
</commit_message>
<xml_diff>
--- a/src/config/datalist.xlsx
+++ b/src/config/datalist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>日期</t>
   </si>
@@ -175,16 +175,7 @@
     <t>关于前端需要知道的一些知识点</t>
   </si>
   <si>
-    <t>2024/3/6</t>
-  </si>
-  <si>
-    <t>eee55544</t>
-  </si>
-  <si>
-    <t>rrrrreeeeessss</t>
-  </si>
-  <si>
-    <t>tsts</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -242,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -261,6 +252,12 @@
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -582,21 +579,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="46.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="55.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="64.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="58.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="46.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="55.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="64.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="58.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +615,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -640,7 +637,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -662,7 +659,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75" customFormat="1" s="5">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +681,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21.75" customFormat="1" s="5">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -706,7 +703,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21.75">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -728,7 +725,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21.75">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -750,7 +747,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21.75">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -772,7 +769,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21.75">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -794,7 +791,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="21.75">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -816,7 +813,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21.75">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -838,7 +835,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21.75">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -860,7 +857,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21.75">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -882,7 +879,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21.75">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -904,7 +901,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21.75">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -926,18 +923,16 @@
       <c r="K15" s="3"/>
       <c r="L15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21.75">
+      <c r="A16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
+      <c r="B16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
@@ -948,8 +943,8 @@
       <c r="K16" s="3"/>
       <c r="L16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="7"/>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21.75">
+      <c r="A17" s="9"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -962,8 +957,8 @@
       <c r="K17" s="3"/>
       <c r="L17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="7"/>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="21.75">
+      <c r="A18" s="9"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -976,8 +971,8 @@
       <c r="K18" s="3"/>
       <c r="L18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="7"/>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21.75">
+      <c r="A19" s="9"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -990,8 +985,8 @@
       <c r="K19" s="3"/>
       <c r="L19" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="7"/>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="21.75">
+      <c r="A20" s="9"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1004,8 +999,8 @@
       <c r="K20" s="3"/>
       <c r="L20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="7"/>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="21.75">
+      <c r="A21" s="9"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1018,8 +1013,8 @@
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="7"/>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="21.75">
+      <c r="A22" s="9"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1032,8 +1027,8 @@
       <c r="K22" s="3"/>
       <c r="L22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="7"/>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="21.75">
+      <c r="A23" s="9"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1046,8 +1041,8 @@
       <c r="K23" s="3"/>
       <c r="L23" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="7"/>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="21.75">
+      <c r="A24" s="9"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1060,8 +1055,8 @@
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="7"/>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="21.75">
+      <c r="A25" s="9"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1074,8 +1069,8 @@
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="7"/>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="21.75">
+      <c r="A26" s="9"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1089,7 +1084,7 @@
       <c r="L26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="21.75">
-      <c r="A27" s="7"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1103,7 +1098,7 @@
       <c r="L27" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="21.75">
-      <c r="A28" s="7"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1117,7 +1112,7 @@
       <c r="L28" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="21.75">
-      <c r="A29" s="7"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1131,7 +1126,7 @@
       <c r="L29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="21.75">
-      <c r="A30" s="7"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1145,7 +1140,7 @@
       <c r="L30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="21.75">
-      <c r="A31" s="7"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1159,7 +1154,7 @@
       <c r="L31" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="21.75">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1173,7 +1168,7 @@
       <c r="L32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="21.75">
-      <c r="A33" s="7"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1187,7 +1182,7 @@
       <c r="L33" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1201,7 +1196,7 @@
       <c r="L34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1215,7 +1210,7 @@
       <c r="L35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1229,7 +1224,7 @@
       <c r="L36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
-      <c r="A37" s="7"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1243,7 +1238,7 @@
       <c r="L37" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
-      <c r="A38" s="7"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1257,7 +1252,7 @@
       <c r="L38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
-      <c r="A39" s="7"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1271,7 +1266,7 @@
       <c r="L39" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
-      <c r="A40" s="7"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1285,7 +1280,7 @@
       <c r="L40" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
-      <c r="A41" s="7"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1299,7 +1294,7 @@
       <c r="L41" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
-      <c r="A42" s="7"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1313,7 +1308,7 @@
       <c r="L42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1327,7 +1322,7 @@
       <c r="L43" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1341,7 +1336,7 @@
       <c r="L44" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
-      <c r="A45" s="7"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1355,7 +1350,7 @@
       <c r="L45" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
-      <c r="A46" s="7"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1369,7 +1364,7 @@
       <c r="L46" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
-      <c r="A47" s="7"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1383,7 +1378,7 @@
       <c r="L47" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
-      <c r="A48" s="7"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1397,7 +1392,7 @@
       <c r="L48" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
-      <c r="A49" s="7"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1411,7 +1406,7 @@
       <c r="L49" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
-      <c r="A50" s="7"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -1425,7 +1420,7 @@
       <c r="L50" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
-      <c r="A51" s="7"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>

</xml_diff>